<commit_message>
-4 for number of commands in sr algo
</commit_message>
<xml_diff>
--- a/docs/probability.xlsx
+++ b/docs/probability.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="3705" windowHeight="1170"/>
@@ -12,23 +12,23 @@
     <sheet name="Operators" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="Bytes_to_store_cell_addr">'Full Vocabulary'!$B$41</definedName>
-    <definedName name="Bytes_to_store_command_id">'Full Vocabulary'!$B$38</definedName>
-    <definedName name="Bytes_to_store_direction">'Full Vocabulary'!$B$40</definedName>
-    <definedName name="Bytes_to_store_ref">'Full Vocabulary'!$B$42</definedName>
-    <definedName name="Bytes_to_store_register">'Full Vocabulary'!$B$39</definedName>
-    <definedName name="Commands_in_self_replication_algorithm">'Full Vocabulary'!$B$45</definedName>
-    <definedName name="Gb">'Full Vocabulary'!$B$46</definedName>
-    <definedName name="Kb">'Full Vocabulary'!$B$46</definedName>
-    <definedName name="Number_of_Dir_Registers">'Full Vocabulary'!$B$35</definedName>
-    <definedName name="Number_of_Directions">'Full Vocabulary'!$B$36</definedName>
-    <definedName name="Number_of_Registers">'Full Vocabulary'!$B$34</definedName>
-    <definedName name="Power_of_reg_ref">'Full Vocabulary'!$B$32</definedName>
-    <definedName name="Power_reference">'Full Vocabulary'!$B$33</definedName>
-    <definedName name="size_of_cell">'Full Vocabulary'!$B$37</definedName>
-    <definedName name="Tb">'Full Vocabulary'!$B$47</definedName>
+    <definedName name="Bytes_to_store_cell_addr">'Full Vocabulary'!$B$42</definedName>
+    <definedName name="Bytes_to_store_command_id">'Full Vocabulary'!$B$39</definedName>
+    <definedName name="Bytes_to_store_direction">'Full Vocabulary'!$B$41</definedName>
+    <definedName name="Bytes_to_store_ref">'Full Vocabulary'!$B$43</definedName>
+    <definedName name="Bytes_to_store_register">'Full Vocabulary'!$B$40</definedName>
+    <definedName name="Commands_in_self_replication_algorithm">'Full Vocabulary'!$B$46</definedName>
+    <definedName name="Gb">'Full Vocabulary'!$B$47</definedName>
+    <definedName name="Kb">'Full Vocabulary'!$B$47</definedName>
+    <definedName name="Number_of_Dir_Registers">'Full Vocabulary'!$B$36</definedName>
+    <definedName name="Number_of_Directions">'Full Vocabulary'!$B$37</definedName>
+    <definedName name="Number_of_Registers">'Full Vocabulary'!$B$35</definedName>
+    <definedName name="Power_of_reg_ref">'Full Vocabulary'!$B$33</definedName>
+    <definedName name="Power_reference">'Full Vocabulary'!$B$34</definedName>
+    <definedName name="size_of_cell">'Full Vocabulary'!$B$38</definedName>
+    <definedName name="Tb">'Full Vocabulary'!$B$48</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -242,17 +242,17 @@
     <t>Years to generate (5 ms to generate and check 1 cell)</t>
   </si>
   <si>
-    <t>UnswappableFrom direction, direction</t>
+    <t>SwapCell dir_register, register</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000000000E+00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -329,7 +329,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -342,9 +342,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -382,7 +382,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -416,7 +416,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -451,10 +450,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -627,14 +625,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="49.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.5703125" style="2" customWidth="1"/>
@@ -646,7 +644,7 @@
     <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="B1" s="11" t="s">
         <v>2</v>
       </c>
@@ -657,7 +655,7 @@
       <c r="G1" s="11"/>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -677,32 +675,33 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>59</v>
       </c>
       <c r="B3" s="3">
-        <f>Number_of_Registers * B31</f>
+        <f>Number_of_Registers * B32</f>
         <v>12884901888</v>
       </c>
       <c r="C3" s="3">
-        <f>Number_of_Registers * C31</f>
+        <f>Number_of_Registers * C32</f>
         <v>196608</v>
       </c>
       <c r="D3" s="3">
-        <f>Number_of_Registers * D31</f>
+        <f>Number_of_Registers * D32</f>
         <v>3072</v>
       </c>
       <c r="E3" s="3">
-        <f>Number_of_Registers * E31</f>
+        <f>Number_of_Registers * E32</f>
         <v>768</v>
       </c>
       <c r="F3" s="3">
-        <f>Number_of_Registers * F31</f>
+        <f>Number_of_Registers * F32</f>
         <v>240</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -726,33 +725,34 @@
         <f>Number_of_Registers</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>63</v>
       </c>
       <c r="B5" s="3">
-        <f>Number_of_Registers * B31 * size_of_cell</f>
+        <f>Number_of_Registers * B32 * size_of_cell</f>
         <v>1030792151040</v>
       </c>
       <c r="C5" s="3">
-        <f>Number_of_Registers * C31 * size_of_cell</f>
+        <f>Number_of_Registers * C32 * size_of_cell</f>
         <v>15728640</v>
       </c>
       <c r="D5" s="3">
-        <f>Number_of_Registers * D31 * size_of_cell</f>
+        <f>Number_of_Registers * D32 * size_of_cell</f>
         <v>245760</v>
       </c>
       <c r="E5" s="3">
-        <f>Number_of_Registers * E31 * size_of_cell</f>
+        <f>Number_of_Registers * E32 * size_of_cell</f>
         <v>61440</v>
       </c>
       <c r="F5" s="3">
-        <f>Number_of_Registers * F31 * size_of_cell</f>
+        <f>Number_of_Registers * F32 * size_of_cell</f>
         <v>19200</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -777,7 +777,7 @@
         <v>25920</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>65</v>
       </c>
@@ -802,7 +802,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>60</v>
       </c>
@@ -810,19 +810,19 @@
         <v>1</v>
       </c>
       <c r="C8" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E8" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F8" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>61</v>
       </c>
@@ -847,7 +847,7 @@
         <v>5832</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -855,583 +855,588 @@
         <v>1</v>
       </c>
       <c r="C10" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E10" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F10" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>69</v>
       </c>
       <c r="B11" s="3">
-        <f>Number_of_Directions * Number_of_Directions</f>
-        <v>25</v>
+        <f>Number_of_Dir_Registers * Number_of_Registers</f>
+        <v>3</v>
       </c>
       <c r="C11" s="3">
-        <f>Number_of_Directions * Number_of_Directions</f>
-        <v>25</v>
+        <f>Number_of_Dir_Registers * Number_of_Registers</f>
+        <v>3</v>
       </c>
       <c r="D11" s="3">
-        <f>Number_of_Directions * Number_of_Directions</f>
-        <v>25</v>
+        <f>Number_of_Dir_Registers * Number_of_Registers</f>
+        <v>3</v>
       </c>
       <c r="E11" s="3">
-        <f>Number_of_Directions * Number_of_Directions</f>
-        <v>25</v>
+        <f>Number_of_Dir_Registers * Number_of_Registers</f>
+        <v>3</v>
       </c>
       <c r="F11" s="3">
-        <f>Number_of_Directions * Number_of_Directions</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+        <f>Number_of_Dir_Registers * Number_of_Registers</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="3">
-        <f t="shared" ref="B13:E13" si="0">SUM(B3:B11)</f>
-        <v>1043677084790</v>
-      </c>
-      <c r="C13" s="3">
-        <f t="shared" si="0"/>
-        <v>15957112</v>
-      </c>
-      <c r="D13" s="3">
-        <f t="shared" si="0"/>
-        <v>280698</v>
-      </c>
-      <c r="E13" s="3">
-        <f t="shared" si="0"/>
-        <v>94076</v>
-      </c>
-      <c r="F13" s="3">
+      <c r="B14" s="3">
+        <f>SUM(B3:B11)</f>
+        <v>1043677084768</v>
+      </c>
+      <c r="C14" s="3">
+        <f>SUM(C3:C11)</f>
+        <v>15957088</v>
+      </c>
+      <c r="D14" s="3">
+        <f>SUM(D3:D11)</f>
+        <v>280672</v>
+      </c>
+      <c r="E14" s="3">
+        <f>SUM(E3:E11)</f>
+        <v>94048</v>
+      </c>
+      <c r="F14" s="3">
         <f>SUM(F3:F11)</f>
-        <v>51310</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+        <v>51280</v>
+      </c>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="3">
-        <f t="shared" ref="B14" si="1">B13 / size_of_cell</f>
-        <v>13045963559.875</v>
-      </c>
-      <c r="C14" s="3">
-        <f t="shared" ref="C14:F14" si="2">C13 / size_of_cell</f>
-        <v>199463.9</v>
-      </c>
-      <c r="D14" s="3">
-        <f t="shared" si="2"/>
-        <v>3508.7249999999999</v>
-      </c>
-      <c r="E14" s="3">
-        <f t="shared" si="2"/>
-        <v>1175.95</v>
-      </c>
-      <c r="F14" s="3">
-        <f t="shared" si="2"/>
-        <v>641.375</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="B15" s="3">
+        <f t="shared" ref="B15" si="0">B14 / size_of_cell</f>
+        <v>13045963559.6</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" ref="C15:F15" si="1">C14 / size_of_cell</f>
+        <v>199463.6</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="1"/>
+        <v>3508.4</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="1"/>
+        <v>1175.5999999999999</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="1"/>
+        <v>641</v>
+      </c>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="4">
-        <f t="shared" ref="B15" si="3">POWER(1 / B13, Commands_in_self_replication_algorithm)</f>
-        <v>0</v>
-      </c>
-      <c r="C15" s="4">
-        <f t="shared" ref="C15:F15" si="4">POWER(1 / C13, Commands_in_self_replication_algorithm)</f>
-        <v>2.0762506817997142E-202</v>
-      </c>
-      <c r="D15" s="4">
+      <c r="B16" s="4">
+        <f t="shared" ref="B16" si="2">POWER(1 / B14, Commands_in_self_replication_algorithm)</f>
+        <v>3.5843667973533758E-289</v>
+      </c>
+      <c r="C16" s="4">
+        <f t="shared" ref="C16:F16" si="3">POWER(1 / C14, Commands_in_self_replication_algorithm)</f>
+        <v>1.3462094592594958E-173</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" si="3"/>
+        <v>1.7507408132084053E-131</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" si="3"/>
+        <v>4.3612446989874965E-120</v>
+      </c>
+      <c r="F16" s="4">
+        <f>POWER(1 / F14, Commands_in_self_replication_algorithm)</f>
+        <v>9.1463455224325951E-114</v>
+      </c>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="4">
+        <f>POWER(B14,Commands_in_self_replication_algorithm)</f>
+        <v>2.7898930453724227E+288</v>
+      </c>
+      <c r="C17" s="4">
+        <f>POWER(C14,Commands_in_self_replication_algorithm)</f>
+        <v>7.4282645477031992E+172</v>
+      </c>
+      <c r="D17" s="4">
+        <f>POWER(D14,Commands_in_self_replication_algorithm)</f>
+        <v>5.7118677559552681E+130</v>
+      </c>
+      <c r="E17" s="4">
+        <f>POWER(E14,Commands_in_self_replication_algorithm)</f>
+        <v>2.2929233946266709E+119</v>
+      </c>
+      <c r="F17" s="4">
+        <f>POWER(F14,Commands_in_self_replication_algorithm)</f>
+        <v>1.0933328481275618E+113</v>
+      </c>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="4">
+        <f>MAX(B22:B29) * size_of_cell * B17 / Tb</f>
+        <v>1.5623401054085566E+279</v>
+      </c>
+      <c r="C18" s="4">
+        <f>MAX(C22:C29) * size_of_cell * C17 / Tb</f>
+        <v>4.1598281467137917E+163</v>
+      </c>
+      <c r="D18" s="4">
+        <f>MAX(D22:D29) * size_of_cell * D17 / Tb</f>
+        <v>3.1986459433349498E+121</v>
+      </c>
+      <c r="E18" s="4">
+        <f>MAX(E22:E29) * size_of_cell * E17 / Tb</f>
+        <v>1.2840371009909357E+110</v>
+      </c>
+      <c r="F18" s="4">
+        <f>MAX(F22:F29) * size_of_cell * F17 / Tb</f>
+        <v>6.1226639495143464E+103</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="4">
+        <f>(B17 * 50) / 1000 / 60 / 60 / 24 / 30 / 12</f>
+        <v>4.4847817730395166E+279</v>
+      </c>
+      <c r="C19" s="4">
+        <f t="shared" ref="C19:E19" si="4">(C17 * 50) / 1000 / 60 / 60 / 24 / 30 / 12</f>
+        <v>1.1941011682907667E+164</v>
+      </c>
+      <c r="D19" s="4">
         <f t="shared" si="4"/>
-        <v>2.8138379901760166E-153</v>
-      </c>
-      <c r="E15" s="4">
+        <v>9.1818861817696565E+121</v>
+      </c>
+      <c r="E19" s="4">
         <f t="shared" si="4"/>
-        <v>5.5283099442523164E-140</v>
-      </c>
-      <c r="F15" s="4">
-        <f t="shared" si="4"/>
-        <v>1.3011986069212942E-132</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="4" t="e">
-        <f>POWER(B13,Commands_in_self_replication_algorithm)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C16" s="4">
-        <f>POWER(C13,Commands_in_self_replication_algorithm)</f>
-        <v>4.8163740957001847E+201</v>
-      </c>
-      <c r="D16" s="4">
-        <f>POWER(D13,Commands_in_self_replication_algorithm)</f>
-        <v>3.5538648759854372E+152</v>
-      </c>
-      <c r="E16" s="4">
-        <f>POWER(E13,Commands_in_self_replication_algorithm)</f>
-        <v>1.8088710837200459E+139</v>
-      </c>
-      <c r="F16" s="4">
-        <f>POWER(F13,Commands_in_self_replication_algorithm)</f>
-        <v>7.6852218768205954E+131</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="4" t="e">
-        <f>MAX(B21:B28) * size_of_cell * B16 / Tb</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C17" s="4">
-        <f>MAX(C21:C28) * size_of_cell * C16 / Tb</f>
-        <v>2.6971694935921033E+192</v>
-      </c>
-      <c r="D17" s="4">
-        <f>MAX(D21:D28) * size_of_cell * D16 / Tb</f>
-        <v>1.990164330551845E+143</v>
-      </c>
-      <c r="E17" s="4">
-        <f>MAX(E21:E28) * size_of_cell * E16 / Tb</f>
-        <v>1.0129678068832258E+130</v>
-      </c>
-      <c r="F17" s="4">
-        <f>MAX(F21:F28) * size_of_cell * F16 / Tb</f>
-        <v>4.3037242510195335E+122</v>
-      </c>
-      <c r="I17" s="4"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B18" s="4" t="e">
-        <f>(B16 * 50) / 1000 / 60 / 60 / 24 / 30 / 12</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C18" s="4">
-        <f t="shared" ref="C18:E18" si="5">(C16 * 50) / 1000 / 60 / 60 / 24 / 30 / 12</f>
-        <v>7.742370910011871E+192</v>
-      </c>
-      <c r="D18" s="4">
-        <f t="shared" si="5"/>
-        <v>5.7128743505424347E+143</v>
-      </c>
-      <c r="E18" s="4">
-        <f t="shared" si="5"/>
-        <v>2.907778876864786E+130</v>
-      </c>
-      <c r="F18" s="4">
-        <f>(F16 * 5) / 1000 / 60 / 60 / 24 / 30 / 12</f>
-        <v>1.2354073233057801E+122</v>
-      </c>
-      <c r="G18" s="2" t="s">
+        <v>3.6858979466092321E+110</v>
+      </c>
+      <c r="F19" s="4">
+        <f>(F17 * 5) / 1000 / 60 / 60 / 24 / 30 / 12</f>
+        <v>1.7575438016453863E+103</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="I18" s="5"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I19" s="6"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="8" t="s">
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="I20" s="6"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="1"/>
+      <c r="B21" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" t="s">
         <v>59</v>
       </c>
-      <c r="B21" s="2">
-        <f>Bytes_to_store_command_id + Bytes_to_store_register + B43</f>
+      <c r="B22" s="2">
+        <f>Bytes_to_store_command_id + Bytes_to_store_register + B44</f>
         <v>6</v>
       </c>
-      <c r="C21" s="2">
-        <f>Bytes_to_store_command_id + Bytes_to_store_register + C43</f>
+      <c r="C22" s="2">
+        <f>Bytes_to_store_command_id + Bytes_to_store_register + C44</f>
         <v>4</v>
       </c>
-      <c r="D21" s="2">
-        <f>Bytes_to_store_command_id + Bytes_to_store_register + D43</f>
+      <c r="D22" s="2">
+        <f>Bytes_to_store_command_id + Bytes_to_store_register + D44</f>
         <v>4</v>
       </c>
-      <c r="E21" s="2">
-        <f>Bytes_to_store_command_id + Bytes_to_store_register + E43</f>
+      <c r="E22" s="2">
+        <f>Bytes_to_store_command_id + Bytes_to_store_register + E44</f>
         <v>3</v>
       </c>
-      <c r="F21" s="2">
-        <f>Bytes_to_store_command_id + Bytes_to_store_register + F43</f>
+      <c r="F22" s="2">
+        <f>Bytes_to_store_command_id + Bytes_to_store_register + F44</f>
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="23" spans="1:9">
+      <c r="A23" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B23" s="2">
         <f>Bytes_to_store_command_id + Bytes_to_store_register</f>
         <v>2</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C23" s="2">
         <f>Bytes_to_store_command_id + Bytes_to_store_register</f>
         <v>2</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D23" s="2">
         <f>Bytes_to_store_command_id + Bytes_to_store_register</f>
         <v>2</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E23" s="2">
         <f>Bytes_to_store_command_id + Bytes_to_store_register</f>
         <v>2</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F23" s="2">
         <f>Bytes_to_store_command_id + Bytes_to_store_register</f>
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="24" spans="1:9">
+      <c r="A24" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="2">
-        <f>Bytes_to_store_command_id + Bytes_to_store_register + B43 + Bytes_to_store_cell_addr</f>
+      <c r="B24" s="2">
+        <f>Bytes_to_store_command_id + Bytes_to_store_register + B44 + Bytes_to_store_cell_addr</f>
         <v>7</v>
       </c>
-      <c r="C23" s="2">
-        <f>Bytes_to_store_command_id + Bytes_to_store_register + C43 + Bytes_to_store_cell_addr</f>
+      <c r="C24" s="2">
+        <f>Bytes_to_store_command_id + Bytes_to_store_register + C44 + Bytes_to_store_cell_addr</f>
         <v>5</v>
       </c>
-      <c r="D23" s="2">
-        <f>Bytes_to_store_command_id + Bytes_to_store_register + D43 + Bytes_to_store_cell_addr</f>
+      <c r="D24" s="2">
+        <f>Bytes_to_store_command_id + Bytes_to_store_register + D44 + Bytes_to_store_cell_addr</f>
         <v>5</v>
       </c>
-      <c r="E23" s="2">
-        <f>Bytes_to_store_command_id + Bytes_to_store_register + E43 + Bytes_to_store_cell_addr</f>
+      <c r="E24" s="2">
+        <f>Bytes_to_store_command_id + Bytes_to_store_register + E44 + Bytes_to_store_cell_addr</f>
         <v>4</v>
       </c>
-      <c r="F23" s="2">
-        <f>Bytes_to_store_command_id + Bytes_to_store_register + F43 + Bytes_to_store_cell_addr</f>
+      <c r="F24" s="2">
+        <f>Bytes_to_store_command_id + Bytes_to_store_register + F44 + Bytes_to_store_cell_addr</f>
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
         <v>64</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B25" s="2">
         <f>Bytes_to_store_command_id + Bytes_to_store_ref + Bytes_to_store_ref + Bytes_to_store_cell_addr</f>
         <v>6</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C25" s="2">
         <f>Bytes_to_store_command_id + Bytes_to_store_ref + Bytes_to_store_ref + Bytes_to_store_cell_addr</f>
         <v>6</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D25" s="2">
         <f>Bytes_to_store_command_id + Bytes_to_store_ref + Bytes_to_store_ref + Bytes_to_store_cell_addr</f>
         <v>6</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E25" s="2">
         <f>Bytes_to_store_command_id + Bytes_to_store_ref + Bytes_to_store_ref + Bytes_to_store_cell_addr</f>
         <v>6</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F25" s="2">
         <f>Bytes_to_store_command_id + Bytes_to_store_ref + Bytes_to_store_ref + Bytes_to_store_cell_addr</f>
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="26" spans="1:9">
+      <c r="A26" t="s">
         <v>65</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B26" s="2">
         <f>Bytes_to_store_command_id + Bytes_to_store_cell_addr</f>
         <v>2</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C26" s="2">
         <f>Bytes_to_store_command_id + Bytes_to_store_cell_addr</f>
         <v>2</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D26" s="2">
         <f>Bytes_to_store_command_id + Bytes_to_store_cell_addr</f>
         <v>2</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E26" s="2">
         <f>Bytes_to_store_command_id + Bytes_to_store_cell_addr</f>
         <v>2</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F26" s="2">
         <f>Bytes_to_store_command_id + Bytes_to_store_cell_addr</f>
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="27" spans="1:9">
+      <c r="A27" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B27" s="2">
         <f>Bytes_to_store_command_id + Bytes_to_store_register</f>
         <v>2</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C27" s="2">
         <f>Bytes_to_store_command_id + Bytes_to_store_register</f>
         <v>2</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D27" s="2">
         <f>Bytes_to_store_command_id + Bytes_to_store_register</f>
         <v>2</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E27" s="2">
         <f>Bytes_to_store_command_id + Bytes_to_store_register</f>
         <v>2</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F27" s="2">
         <f>Bytes_to_store_command_id + Bytes_to_store_register</f>
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="28" spans="1:9">
+      <c r="A28" t="s">
         <v>61</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B28" s="2">
         <f>Bytes_to_store_command_id + Bytes_to_store_ref * 3</f>
         <v>7</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C28" s="2">
         <f>Bytes_to_store_command_id + Bytes_to_store_ref * 3</f>
         <v>7</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D28" s="2">
         <f>Bytes_to_store_command_id + Bytes_to_store_ref * 3</f>
         <v>7</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E28" s="2">
         <f>Bytes_to_store_command_id + Bytes_to_store_ref * 3</f>
         <v>7</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F28" s="2">
         <f>Bytes_to_store_command_id + Bytes_to_store_ref * 3</f>
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="29" spans="1:9">
+      <c r="A29" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B29" s="2">
         <f>Bytes_to_store_command_id</f>
         <v>1</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C29" s="2">
         <f>Bytes_to_store_command_id</f>
         <v>1</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D29" s="2">
         <f>Bytes_to_store_command_id</f>
         <v>1</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E29" s="2">
         <f>Bytes_to_store_command_id</f>
         <v>1</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F29" s="2">
         <f>Bytes_to_store_command_id</f>
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    <row r="31" spans="1:9">
+      <c r="A31" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="32" spans="1:9">
+      <c r="A32" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B32" s="2">
         <f>POWER(2,B2)</f>
         <v>4294967296</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C32" s="2">
         <f>POWER(2,C2)</f>
         <v>65536</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D32" s="2">
         <f>POWER(2,D2)</f>
         <v>1024</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E32" s="2">
         <f>POWER(2,E2)</f>
         <v>256</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F32" s="2">
         <f>size_of_cell</f>
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
         <v>56</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B33" s="2">
         <f>Number_of_Directions * Number_of_Registers</f>
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B34" s="2">
         <f>(Number_of_Directions + Number_of_Dir_Registers) * Number_of_Registers</f>
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B35" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
         <v>62</v>
       </c>
-      <c r="B35" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="B36" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B37" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B38" s="2">
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
         <v>11</v>
       </c>
-      <c r="B38" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="B39" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
         <v>12</v>
       </c>
-      <c r="B39" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="B40" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
         <v>15</v>
       </c>
-      <c r="B40" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="B41" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
         <v>16</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B42" s="2">
         <f>ROUNDUP(LOG(size_of_cell,2) / 8,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
         <v>14</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B43" s="2">
         <f>Bytes_to_store_direction + Bytes_to_store_register</f>
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
         <v>13</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B44" s="2">
         <f>ROUNDUP(B2/8,0)</f>
         <v>4</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C44" s="2">
         <f>ROUNDUP(C2/8,0)</f>
         <v>2</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D44" s="2">
         <f>ROUNDUP(D2/8,0)</f>
         <v>2</v>
       </c>
-      <c r="E43" s="2">
+      <c r="E44" s="2">
         <f>ROUNDUP(E2/8,0)</f>
         <v>1</v>
       </c>
-      <c r="F43" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="F44" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
         <v>20</v>
       </c>
-      <c r="B45" s="2">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="B46" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
         <v>17</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B47" s="2">
         <f>1000 * 1000 * 1000</f>
         <v>1000000000</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="48" spans="1:6">
+      <c r="A48" t="s">
         <v>21</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B48" s="2">
         <f>1000 * Gb</f>
         <v>1000000000000</v>
       </c>
@@ -1446,21 +1451,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="69.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -1472,27 +1477,27 @@
         <v>240</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="9" t="s">
         <v>25</v>
       </c>
@@ -1504,17 +1509,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="9" t="s">
         <v>27</v>
       </c>
@@ -1526,27 +1531,27 @@
         <v>19200</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" s="9" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" s="9" t="s">
         <v>30</v>
       </c>
@@ -1558,27 +1563,27 @@
         <v>18000</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="A20" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" s="9" t="s">
         <v>39</v>
       </c>
@@ -1586,7 +1591,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="A26" s="9" t="s">
         <v>43</v>
       </c>
@@ -1598,30 +1603,30 @@
         <v>225</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27" s="9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="A28" s="9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="A29" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="A30" s="9" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7">
       <c r="A32" s="9"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" s="9" t="s">
         <v>49</v>
       </c>
@@ -1633,7 +1638,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -1648,14 +1653,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>

</xml_diff>